<commit_message>
had to fix some date errors in original data
</commit_message>
<xml_diff>
--- a/Finance_Data/2019/Dec_2019.xlsx
+++ b/Finance_Data/2019/Dec_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\Desktop\Finance_Analysis_PowerBI\Finance_Data\2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3017B7D1-CEBC-4752-A70D-53342E9BDFF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402C7703-E91F-4FBA-BE94-BAB0961FD08C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-660" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44166</v>
+        <v>43800</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>44178</v>
+        <v>43812</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>44193</v>
+        <v>43827</v>
       </c>
       <c r="B52" t="s">
         <v>44</v>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>44191</v>
+        <v>43825</v>
       </c>
       <c r="B53" t="s">
         <v>44</v>

</xml_diff>